<commit_message>
create file upload-giangvien.ejs (template)
</commit_message>
<xml_diff>
--- a/docs/TemplateOffices/xlxs/giangvien.xlsx
+++ b/docs/TemplateOffices/xlxs/giangvien.xlsx
@@ -103,46 +103,46 @@
     <t>huanhx@vnu.edu.vn</t>
   </si>
   <si>
+    <t>fit002</t>
+  </si>
+  <si>
+    <t>fit003</t>
+  </si>
+  <si>
+    <t>fit004</t>
+  </si>
+  <si>
+    <t>fit005</t>
+  </si>
+  <si>
+    <t>fit006</t>
+  </si>
+  <si>
+    <t>fot007</t>
+  </si>
+  <si>
+    <t>fit008</t>
+  </si>
+  <si>
+    <t>fit009</t>
+  </si>
+  <si>
+    <t>fit010</t>
+  </si>
+  <si>
+    <t>fit011</t>
+  </si>
+  <si>
+    <t>fit012</t>
+  </si>
+  <si>
+    <t>fit013</t>
+  </si>
+  <si>
+    <t>DonViId</t>
+  </si>
+  <si>
     <t>fit001</t>
-  </si>
-  <si>
-    <t>fit002</t>
-  </si>
-  <si>
-    <t>fit003</t>
-  </si>
-  <si>
-    <t>fit004</t>
-  </si>
-  <si>
-    <t>fit005</t>
-  </si>
-  <si>
-    <t>fit006</t>
-  </si>
-  <si>
-    <t>fot007</t>
-  </si>
-  <si>
-    <t>fit008</t>
-  </si>
-  <si>
-    <t>fit009</t>
-  </si>
-  <si>
-    <t>fit010</t>
-  </si>
-  <si>
-    <t>fit011</t>
-  </si>
-  <si>
-    <t>fit012</t>
-  </si>
-  <si>
-    <t>fit013</t>
-  </si>
-  <si>
-    <t>DonViId</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,12 +541,12 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>27</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>13</v>

</xml_diff>